<commit_message>
calculate fairness results (for 1QUICvs2TCP & 1QUICvs5TCP)
</commit_message>
<xml_diff>
--- a/Results/DLT - 10 simulations average.xlsx
+++ b/Results/DLT - 10 simulations average.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/muhammadeid/Desktop/QUIC-vs-TCP-A-Performance-Evaluation-over-LTE-with-NS-3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/muhammadeid/Desktop/waqs/QUIC-vs-TCP-A-Performance-Evaluation-over-LTE-with-NS-3/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE1D4FC8-E486-714D-B8D4-621A3C5BDCA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C6F7329-6C36-1E46-B59E-742EECBDE815}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17520" xr2:uid="{F39ACBC6-E416-9A48-862C-2D5A23947300}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19620" xr2:uid="{F39ACBC6-E416-9A48-862C-2D5A23947300}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,15 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
-    <t>Avg. TCP Throughput (Mbps)</t>
-  </si>
-  <si>
-    <t>Avg. QUIC Throughput (Mbps)</t>
-  </si>
-  <si>
-    <t>Distance from eNB (m)</t>
-  </si>
-  <si>
     <t>64KB</t>
   </si>
   <si>
@@ -66,6 +57,15 @@
   </si>
   <si>
     <t>Reduction (%)</t>
+  </si>
+  <si>
+    <t>Avg. TCP DLT (Mbps)</t>
+  </si>
+  <si>
+    <t>Avg. QUIC DLT (Mbps)</t>
+  </si>
+  <si>
+    <t>File Size</t>
   </si>
 </sst>
 </file>
@@ -179,7 +179,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Avg. TCP Throughput (Mbps)</c:v>
+                  <c:v>Avg. TCP DLT (Mbps)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -248,7 +248,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Avg. QUIC Throughput (Mbps)</c:v>
+                  <c:v>Avg. QUIC DLT (Mbps)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1393,9 +1393,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28C5CC41-2414-4345-B181-FE8F3407EF9B}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1407,43 +1405,43 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>3.4</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>3.76</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>4.38</v>
@@ -1458,7 +1456,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>6.62</v>
@@ -1473,7 +1471,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>17.600000000000001</v>

</xml_diff>